<commit_message>
Add bug report, test plan, readme
</commit_message>
<xml_diff>
--- a/doc/bug-report.xlsx
+++ b/doc/bug-report.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="107">
   <si>
     <t>P0 = crash bug, P1 = game stopping but not crash, P2 = not working as expected, P3 = annoying, P4 = nice to have, P5 = future release</t>
   </si>
@@ -156,12 +156,6 @@
     <t>press D -&gt; die to an enemy -&gt; (game restarts) -&gt; release D -&gt; starts moving left</t>
   </si>
   <si>
-    <t>open</t>
-  </si>
-  <si>
-    <t>Will</t>
-  </si>
-  <si>
     <t>collision system sliding on the wall is jittery. when sliding beside the wall and spam movement to move towards the wall, it will jitter and sometimes stop the player</t>
   </si>
   <si>
@@ -184,6 +178,9 @@
   </si>
   <si>
     <t>object in front of player -&gt; hold W -&gt; collide -&gt; hold S or D -&gt; can't go around object</t>
+  </si>
+  <si>
+    <t>open</t>
   </si>
   <si>
     <t>upon player death, player actions like firing, getting hit are still available. there is still a hit sound</t>
@@ -220,6 +217,123 @@
   </si>
   <si>
     <t>Have 2 bullets hit the player in a short time span, shorter than the player invunerbility</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>game engine is rendering every single tile, which causes lag if the map is large</t>
+  </si>
+  <si>
+    <t>should not lag if world is large</t>
+  </si>
+  <si>
+    <t>it is lagging with massive frame drops</t>
+  </si>
+  <si>
+    <t>change world size to 30x30 or larger, upon starting the game, low framerates occur</t>
+  </si>
+  <si>
+    <t>P3</t>
+  </si>
+  <si>
+    <t>heart ui is disappearing due to new render optimization, in order to fix this, introduce renderrequest layers</t>
+  </si>
+  <si>
+    <t>hearts in ui should not disappear when zooming in to the max</t>
+  </si>
+  <si>
+    <t>heart disappears if zoomed in</t>
+  </si>
+  <si>
+    <t>zoom in -&gt; hearts disappear</t>
+  </si>
+  <si>
+    <t>Alan</t>
+  </si>
+  <si>
+    <t>Enemies can cross the wall rather than collide with it</t>
+  </si>
+  <si>
+    <t>enemy should collide with the wall and slide against it</t>
+  </si>
+  <si>
+    <t>enemy cross wall and glitches through it</t>
+  </si>
+  <si>
+    <t>start game -&gt; wait for enemies to spawn and move towards the wall</t>
+  </si>
+  <si>
+    <t>FPS may drop when many enemies are generated. This may be caused by multiple direction calculation to player</t>
+  </si>
+  <si>
+    <t>game should not lag when there are many enemies on the screen</t>
+  </si>
+  <si>
+    <t>game lags when multiple enemies are on the screen</t>
+  </si>
+  <si>
+    <t>start game -&gt; wait for enemies to spawn -&gt; lag occurs when many enemies</t>
+  </si>
+  <si>
+    <t>Alan &amp; Kevin</t>
+  </si>
+  <si>
+    <t>player can phase through anything and get to an unreachable position</t>
+  </si>
+  <si>
+    <t>player should be colliding with the wall after restoring window position</t>
+  </si>
+  <si>
+    <t>player teleports outside of the walls and over the walls</t>
+  </si>
+  <si>
+    <t>hold a direction key near a wall but don't collide with it -&gt; click the window bar and drag it a little to freeze the screen -&gt; unhold the mouse button -&gt; player teleports to the other side</t>
+  </si>
+  <si>
+    <t>since walls have half the collision, enemies can go into a wall tile and be stuck there</t>
+  </si>
+  <si>
+    <t>enemy should not be stuck and perhaps seek a path around the wall if current tile is a wall</t>
+  </si>
+  <si>
+    <t>enemy is stuck trying to get through the wall but can't due to collision</t>
+  </si>
+  <si>
+    <t>let enemy follow player -&gt; go to a wall that has half collision box -&gt; go to other side -&gt; enemy can't move</t>
+  </si>
+  <si>
+    <t>buggy ai. sometimes the path finding stops early when enemy can see the player, this results in it shooting the wall</t>
+  </si>
+  <si>
+    <t>enemy should not stop early and does not shoot the wall</t>
+  </si>
+  <si>
+    <t xml:space="preserve">problem could be from: can see player function. what happens is that in diagonal tiles, it assumes it is on the tile without considering offset. so it shoots the wall </t>
+  </si>
+  <si>
+    <t>make enemy follow to a wall in the middle -&gt; go diagonal from it on the other side, it starts shooting the wall</t>
+  </si>
+  <si>
+    <t>Player being either bounce away from the wall or stuck in the wall when their collider is shifted</t>
+  </si>
+  <si>
+    <t>Player stops at the wall. Do not bounce off or stuck in the wall</t>
+  </si>
+  <si>
+    <t>start game -&gt; press wasd to walk to wall -&gt; player collide the wall</t>
+  </si>
+  <si>
+    <t>player bullets are hitting the wall and disppearing when standing on the top tile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">player bullet should shoot outside and not disappear </t>
+  </si>
+  <si>
+    <t>player bullet is disappearing when firing</t>
+  </si>
+  <si>
+    <t>walk to the top wall tile -&gt; put mouse cursor below the player sprite -&gt; hold left mouse button to fire -&gt; bullet disappears</t>
   </si>
 </sst>
 </file>
@@ -531,6 +645,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1056,22 +1171,22 @@
         <v>13</v>
       </c>
       <c r="E13" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="F13" s="9" t="s">
+      <c r="H13" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="I13" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="H13" s="9" t="s">
+      <c r="J13" s="9" t="s">
         <v>50</v>
-      </c>
-      <c r="I13" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="J13" s="9" t="s">
-        <v>52</v>
       </c>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
@@ -1104,20 +1219,22 @@
         <v>13</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>47</v>
+        <v>14</v>
       </c>
-      <c r="F14" s="3"/>
+      <c r="F14" s="9" t="s">
+        <v>15</v>
+      </c>
       <c r="G14" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="I14" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="H14" s="9" t="s">
+      <c r="J14" s="9" t="s">
         <v>54</v>
-      </c>
-      <c r="I14" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="J14" s="9" t="s">
-        <v>56</v>
       </c>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
@@ -1147,23 +1264,23 @@
         <v>12</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="H15" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="H15" s="9" t="s">
+      <c r="I15" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="I15" s="9" t="s">
+      <c r="J15" s="9" t="s">
         <v>59</v>
-      </c>
-      <c r="J15" s="9" t="s">
-        <v>60</v>
       </c>
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
@@ -1193,23 +1310,23 @@
         <v>12</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="H16" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="H16" s="9" t="s">
+      <c r="I16" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="I16" s="9" t="s">
+      <c r="J16" s="9" t="s">
         <v>63</v>
-      </c>
-      <c r="J16" s="9" t="s">
-        <v>64</v>
       </c>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
@@ -1242,20 +1359,20 @@
         <v>32</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="H17" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="H17" s="9" t="s">
+      <c r="I17" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="I17" s="9" t="s">
+      <c r="J17" s="9" t="s">
         <v>67</v>
-      </c>
-      <c r="J17" s="9" t="s">
-        <v>68</v>
       </c>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
@@ -1275,16 +1392,36 @@
       <c r="Z17" s="3"/>
     </row>
     <row r="18">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
+      <c r="A18" s="9">
+        <v>13.0</v>
+      </c>
+      <c r="B18" s="10">
+        <v>45345.0</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="J18" s="9" t="s">
+        <v>72</v>
+      </c>
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
@@ -1303,16 +1440,34 @@
       <c r="Z18" s="3"/>
     </row>
     <row r="19">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
+      <c r="A19" s="9">
+        <v>14.0</v>
+      </c>
+      <c r="B19" s="10">
+        <v>45349.0</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>55</v>
+      </c>
       <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
+      <c r="G19" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="I19" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="J19" s="9" t="s">
+        <v>77</v>
+      </c>
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
       <c r="M19" s="3"/>
@@ -1331,16 +1486,36 @@
       <c r="Z19" s="3"/>
     </row>
     <row r="20">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
+      <c r="A20" s="9">
+        <v>15.0</v>
+      </c>
+      <c r="B20" s="10">
+        <v>45352.0</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="I20" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="J20" s="9" t="s">
+        <v>82</v>
+      </c>
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
@@ -1359,16 +1534,34 @@
       <c r="Z20" s="3"/>
     </row>
     <row r="21">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
+      <c r="A21" s="9">
+        <v>16.0</v>
+      </c>
+      <c r="B21" s="10">
+        <v>45352.0</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>55</v>
+      </c>
       <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
+      <c r="G21" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="H21" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="I21" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="J21" s="9" t="s">
+        <v>86</v>
+      </c>
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
@@ -1387,16 +1580,34 @@
       <c r="Z21" s="3"/>
     </row>
     <row r="22">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
+      <c r="A22" s="9">
+        <v>17.0</v>
+      </c>
+      <c r="B22" s="10">
+        <v>45354.0</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>55</v>
+      </c>
       <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
+      <c r="G22" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="H22" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="I22" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="J22" s="9" t="s">
+        <v>91</v>
+      </c>
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
@@ -1415,16 +1626,34 @@
       <c r="Z22" s="3"/>
     </row>
     <row r="23">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
+      <c r="A23" s="9">
+        <v>18.0</v>
+      </c>
+      <c r="B23" s="10">
+        <v>45354.0</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>55</v>
+      </c>
       <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
+      <c r="G23" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="H23" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="I23" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="J23" s="9" t="s">
+        <v>95</v>
+      </c>
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
@@ -1443,16 +1672,34 @@
       <c r="Z23" s="3"/>
     </row>
     <row r="24">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
+      <c r="A24" s="9">
+        <v>19.0</v>
+      </c>
+      <c r="B24" s="10">
+        <v>45355.0</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>55</v>
+      </c>
       <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
+      <c r="G24" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="H24" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="I24" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="J24" s="9" t="s">
+        <v>99</v>
+      </c>
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
       <c r="M24" s="3"/>
@@ -1471,16 +1718,36 @@
       <c r="Z24" s="3"/>
     </row>
     <row r="25">
-      <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
+      <c r="A25" s="9">
+        <v>20.0</v>
+      </c>
+      <c r="B25" s="10">
+        <v>45356.0</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G25" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="H25" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="I25" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="J25" s="9" t="s">
+        <v>102</v>
+      </c>
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
       <c r="M25" s="3"/>
@@ -1499,16 +1766,34 @@
       <c r="Z25" s="3"/>
     </row>
     <row r="26">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
+      <c r="A26" s="9">
+        <v>21.0</v>
+      </c>
+      <c r="B26" s="10">
+        <v>45356.0</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>55</v>
+      </c>
       <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
+      <c r="G26" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="H26" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="I26" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="J26" s="9" t="s">
+        <v>106</v>
+      </c>
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
       <c r="M26" s="3"/>
@@ -1527,7 +1812,9 @@
       <c r="Z26" s="3"/>
     </row>
     <row r="27">
-      <c r="A27" s="3"/>
+      <c r="A27" s="9">
+        <v>22.0</v>
+      </c>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
@@ -28802,6 +29089,9 @@
   <mergeCells count="1">
     <mergeCell ref="A3:B3"/>
   </mergeCells>
+  <printOptions gridLines="1" horizontalCentered="1"/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup fitToHeight="0" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix rendering issue and add bug report/test plan
</commit_message>
<xml_diff>
--- a/doc/bug-report.xlsx
+++ b/doc/bug-report.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="129">
   <si>
     <t>P0 = crash bug, P1 = game stopping but not crash, P2 = not working as expected, P3 = annoying, P4 = nice to have, P5 = future release</t>
   </si>
@@ -180,6 +180,9 @@
     <t>object in front of player -&gt; hold W -&gt; collide -&gt; hold S or D -&gt; can't go around object</t>
   </si>
   <si>
+    <t>?</t>
+  </si>
+  <si>
     <t>upon player death, player actions like firing, getting hit are still available. there is still a hit sound</t>
   </si>
   <si>
@@ -204,7 +207,7 @@
     <t>Die while constantly firing</t>
   </si>
   <si>
-    <t>open</t>
+    <t>won't fix</t>
   </si>
   <si>
     <t>During player invunderability, other bullets pass through the player.</t>
@@ -277,6 +280,9 @@
   </si>
   <si>
     <t>Alan &amp; Kevin</t>
+  </si>
+  <si>
+    <t>open</t>
   </si>
   <si>
     <t>player can phase through anything and get to an unreachable position</t>
@@ -370,6 +376,30 @@
   </si>
   <si>
     <t>Spawn a suicide enemy. Stand still and have the enemy walk towards the player by itself.</t>
+  </si>
+  <si>
+    <t>hearts not being added to the top left corner</t>
+  </si>
+  <si>
+    <t>adding hearts should increase the heart in top left corner to one more</t>
+  </si>
+  <si>
+    <t>a row of hearts is added instead</t>
+  </si>
+  <si>
+    <t>pick up an item that increases hp, row of hearts appear in top left corner</t>
+  </si>
+  <si>
+    <t>decision tree is leaking memory, causing game to crash when closing</t>
+  </si>
+  <si>
+    <t>game should not throw exception when exiting</t>
+  </si>
+  <si>
+    <t>redirects to thrown exception in debug file</t>
+  </si>
+  <si>
+    <t>add "delete root" inside of the decision tree destructor, open game, close game, error</t>
   </si>
 </sst>
 </file>
@@ -1305,18 +1335,20 @@
       <c r="E15" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="F15" s="3"/>
-      <c r="G15" s="9" t="s">
+      <c r="F15" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="H15" s="9" t="s">
+      <c r="G15" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="I15" s="9" t="s">
+      <c r="H15" s="9" t="s">
         <v>57</v>
       </c>
+      <c r="I15" s="9" t="s">
+        <v>58</v>
+      </c>
       <c r="J15" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
@@ -1351,18 +1383,20 @@
       <c r="E16" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="F16" s="3"/>
+      <c r="F16" s="9" t="s">
+        <v>55</v>
+      </c>
       <c r="G16" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="J16" s="9" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
@@ -1395,20 +1429,20 @@
         <v>32</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H17" s="9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I17" s="9" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J17" s="9" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
@@ -1438,7 +1472,7 @@
         <v>15</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E18" s="9" t="s">
         <v>14</v>
@@ -1447,16 +1481,16 @@
         <v>15</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H18" s="9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I18" s="9" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J18" s="9" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
@@ -1486,23 +1520,25 @@
         <v>15</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>63</v>
+        <v>14</v>
       </c>
-      <c r="F19" s="3"/>
+      <c r="F19" s="9" t="s">
+        <v>15</v>
+      </c>
       <c r="G19" s="9" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H19" s="9" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I19" s="9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J19" s="9" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
@@ -1529,7 +1565,7 @@
         <v>45352.0</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D20" s="9" t="s">
         <v>13</v>
@@ -1541,16 +1577,16 @@
         <v>15</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H20" s="9" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I20" s="9" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J20" s="9" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
@@ -1577,26 +1613,28 @@
         <v>45352.0</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>63</v>
+        <v>14</v>
       </c>
-      <c r="F21" s="3"/>
+      <c r="F21" s="9" t="s">
+        <v>79</v>
+      </c>
       <c r="G21" s="9" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H21" s="9" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="I21" s="9" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="J21" s="9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
@@ -1623,26 +1661,26 @@
         <v>45354.0</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D22" s="9" t="s">
         <v>13</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>63</v>
+        <v>89</v>
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="9" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H22" s="9" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="I22" s="9" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="J22" s="9" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
@@ -1672,23 +1710,25 @@
         <v>15</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>63</v>
+        <v>14</v>
       </c>
-      <c r="F23" s="3"/>
+      <c r="F23" s="9" t="s">
+        <v>15</v>
+      </c>
       <c r="G23" s="9" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="H23" s="9" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="I23" s="9" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="J23" s="9" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
@@ -1718,23 +1758,23 @@
         <v>15</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F24" s="3"/>
       <c r="G24" s="9" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="H24" s="9" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="I24" s="9" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="J24" s="9" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
@@ -1761,7 +1801,7 @@
         <v>45356.0</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D25" s="9" t="s">
         <v>32</v>
@@ -1770,19 +1810,19 @@
         <v>14</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G25" s="9" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="H25" s="9" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="I25" s="9" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="J25" s="9" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
@@ -1809,26 +1849,28 @@
         <v>45356.0</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>63</v>
+        <v>14</v>
       </c>
-      <c r="F26" s="3"/>
+      <c r="F26" s="9" t="s">
+        <v>15</v>
+      </c>
       <c r="G26" s="9" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H26" s="9" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="I26" s="9" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="J26" s="9" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
@@ -1861,20 +1903,22 @@
         <v>13</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>63</v>
+        <v>14</v>
       </c>
-      <c r="F27" s="3"/>
+      <c r="F27" s="9" t="s">
+        <v>15</v>
+      </c>
       <c r="G27" s="9" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="H27" s="9" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="I27" s="9" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="J27" s="9" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
@@ -1907,20 +1951,22 @@
         <v>13</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>63</v>
+        <v>14</v>
       </c>
-      <c r="F28" s="3"/>
+      <c r="F28" s="9" t="s">
+        <v>15</v>
+      </c>
       <c r="G28" s="9" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="H28" s="9" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="I28" s="9" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="J28" s="9" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
@@ -1953,22 +1999,22 @@
         <v>13</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>63</v>
+        <v>14</v>
       </c>
       <c r="F29" s="9" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G29" s="9" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="H29" s="9" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="I29" s="9" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="J29" s="9" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
@@ -1988,16 +2034,36 @@
       <c r="Z29" s="3"/>
     </row>
     <row r="30">
-      <c r="A30" s="3"/>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
+      <c r="A30" s="9">
+        <v>25.0</v>
+      </c>
+      <c r="B30" s="10">
+        <v>45373.0</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G30" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="H30" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="I30" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="J30" s="9" t="s">
+        <v>124</v>
+      </c>
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
       <c r="M30" s="3"/>
@@ -2016,16 +2082,36 @@
       <c r="Z30" s="3"/>
     </row>
     <row r="31">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
+      <c r="A31" s="9">
+        <v>26.0</v>
+      </c>
+      <c r="B31" s="10">
+        <v>45375.0</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F31" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G31" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="H31" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="I31" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="J31" s="9" t="s">
+        <v>128</v>
+      </c>
       <c r="K31" s="3"/>
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
@@ -2044,14 +2130,14 @@
       <c r="Z31" s="3"/>
     </row>
     <row r="32">
-      <c r="A32" s="3"/>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
+      <c r="A32" s="9"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
       <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
-      <c r="H32" s="3"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>
       <c r="K32" s="3"/>

</xml_diff>

<commit_message>
Updated to latest docs
</commit_message>
<xml_diff>
--- a/doc/bug-report.xlsx
+++ b/doc/bug-report.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="145">
   <si>
     <t>P0 = crash bug, P1 = game stopping but not crash, P2 = not working as expected, P3 = annoying, P4 = nice to have, P5 = future release</t>
   </si>
@@ -401,13 +401,62 @@
   <si>
     <t>add "delete root" inside of the decision tree destructor, open game, close game, error</t>
   </si>
+  <si>
+    <t>mesh collider not working, box collidable is smaller than mesh, so it won't ever check against mesh</t>
+  </si>
+  <si>
+    <t>bullets passing through mesh should hit the player</t>
+  </si>
+  <si>
+    <t>bullets should damage player when passing through mesh collider</t>
+  </si>
+  <si>
+    <t>press g for debug, let enemy shoot you, dodge by going down while letting bullet grace top half of mesh -&gt; not hitting</t>
+  </si>
+  <si>
+    <t>Sometimes the fog of war does not reveal the entire room</t>
+  </si>
+  <si>
+    <t>Entering a room reveals the entire room</t>
+  </si>
+  <si>
+    <t>Occasionally a corner of the room will be hidden in a triangle shape of shadows. Entering the triangle reveals it as normal</t>
+  </si>
+  <si>
+    <t>Generate a room and corridor such that a door is facing vertically is directly next to a door facing horizontally into the other door. The corresponding room will have the fog bug.</t>
+  </si>
+  <si>
+    <t>Sometimes only three enemies will spawn inside a room causing the player to be stuck in that room as they cannot kill the fourth enemy.</t>
+  </si>
+  <si>
+    <t>All four enemies should be inside a room and interactable.</t>
+  </si>
+  <si>
+    <t>An enemy will be missing in a room in some generations.</t>
+  </si>
+  <si>
+    <t>Keep generating and entering rooms until only 3 enemies are accessable.</t>
+  </si>
+  <si>
+    <t>Game crashing when player's room index is -1 which means its in a corridor, so the array access is invalid</t>
+  </si>
+  <si>
+    <t>the game should not crash</t>
+  </si>
+  <si>
+    <t>game crashes</t>
+  </si>
+  <si>
+    <t>[not able to reproduce]</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
+    <numFmt numFmtId="165" formatCode="mm/dd/yyyy"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -464,7 +513,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -500,6 +549,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1664,7 +1716,7 @@
         <v>88</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>13</v>
+        <v>74</v>
       </c>
       <c r="E22" s="9" t="s">
         <v>89</v>
@@ -2130,16 +2182,34 @@
       <c r="Z31" s="3"/>
     </row>
     <row r="32">
-      <c r="A32" s="9"/>
-      <c r="B32" s="10"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
+      <c r="A32" s="9">
+        <v>27.0</v>
+      </c>
+      <c r="B32" s="10">
+        <v>45380.0</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>89</v>
+      </c>
       <c r="F32" s="3"/>
-      <c r="G32" s="9"/>
-      <c r="H32" s="9"/>
-      <c r="I32" s="3"/>
-      <c r="J32" s="3"/>
+      <c r="G32" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="H32" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="I32" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="J32" s="9" t="s">
+        <v>132</v>
+      </c>
       <c r="K32" s="3"/>
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
@@ -2158,16 +2228,36 @@
       <c r="Z32" s="3"/>
     </row>
     <row r="33">
-      <c r="A33" s="3"/>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
-      <c r="I33" s="3"/>
-      <c r="J33" s="3"/>
+      <c r="A33" s="9">
+        <v>28.0</v>
+      </c>
+      <c r="B33" s="12">
+        <v>45391.0</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="F33" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G33" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="H33" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="I33" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="J33" s="9" t="s">
+        <v>136</v>
+      </c>
       <c r="K33" s="3"/>
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
@@ -2186,16 +2276,36 @@
       <c r="Z33" s="3"/>
     </row>
     <row r="34">
-      <c r="A34" s="3"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="3"/>
-      <c r="H34" s="3"/>
-      <c r="I34" s="3"/>
-      <c r="J34" s="3"/>
+      <c r="A34" s="9">
+        <v>29.0</v>
+      </c>
+      <c r="B34" s="12">
+        <v>45391.0</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="F34" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G34" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="H34" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="I34" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="J34" s="9" t="s">
+        <v>140</v>
+      </c>
       <c r="K34" s="3"/>
       <c r="L34" s="3"/>
       <c r="M34" s="3"/>
@@ -2214,16 +2324,36 @@
       <c r="Z34" s="3"/>
     </row>
     <row r="35">
-      <c r="A35" s="3"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
-      <c r="H35" s="3"/>
-      <c r="I35" s="3"/>
-      <c r="J35" s="3"/>
+      <c r="A35" s="9">
+        <v>30.0</v>
+      </c>
+      <c r="B35" s="12">
+        <v>45391.0</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="F35" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G35" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="H35" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="I35" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="J35" s="9" t="s">
+        <v>144</v>
+      </c>
       <c r="K35" s="3"/>
       <c r="L35" s="3"/>
       <c r="M35" s="3"/>

</xml_diff>

<commit_message>
Merge origin/main into feature/levels
</commit_message>
<xml_diff>
--- a/doc/bug-report.xlsx
+++ b/doc/bug-report.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="145">
   <si>
     <t>P0 = crash bug, P1 = game stopping but not crash, P2 = not working as expected, P3 = annoying, P4 = nice to have, P5 = future release</t>
   </si>
@@ -401,13 +401,62 @@
   <si>
     <t>add "delete root" inside of the decision tree destructor, open game, close game, error</t>
   </si>
+  <si>
+    <t>mesh collider not working, box collidable is smaller than mesh, so it won't ever check against mesh</t>
+  </si>
+  <si>
+    <t>bullets passing through mesh should hit the player</t>
+  </si>
+  <si>
+    <t>bullets should damage player when passing through mesh collider</t>
+  </si>
+  <si>
+    <t>press g for debug, let enemy shoot you, dodge by going down while letting bullet grace top half of mesh -&gt; not hitting</t>
+  </si>
+  <si>
+    <t>Sometimes the fog of war does not reveal the entire room</t>
+  </si>
+  <si>
+    <t>Entering a room reveals the entire room</t>
+  </si>
+  <si>
+    <t>Occasionally a corner of the room will be hidden in a triangle shape of shadows. Entering the triangle reveals it as normal</t>
+  </si>
+  <si>
+    <t>Generate a room and corridor such that a door is facing vertically is directly next to a door facing horizontally into the other door. The corresponding room will have the fog bug.</t>
+  </si>
+  <si>
+    <t>Sometimes only three enemies will spawn inside a room causing the player to be stuck in that room as they cannot kill the fourth enemy.</t>
+  </si>
+  <si>
+    <t>All four enemies should be inside a room and interactable.</t>
+  </si>
+  <si>
+    <t>An enemy will be missing in a room in some generations.</t>
+  </si>
+  <si>
+    <t>Keep generating and entering rooms until only 3 enemies are accessable.</t>
+  </si>
+  <si>
+    <t>Game crashing when player's room index is -1 which means its in a corridor, so the array access is invalid</t>
+  </si>
+  <si>
+    <t>the game should not crash</t>
+  </si>
+  <si>
+    <t>game crashes</t>
+  </si>
+  <si>
+    <t>[not able to reproduce]</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
+    <numFmt numFmtId="165" formatCode="mm/dd/yyyy"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -464,7 +513,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -500,6 +549,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1664,7 +1716,7 @@
         <v>88</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>13</v>
+        <v>74</v>
       </c>
       <c r="E22" s="9" t="s">
         <v>89</v>
@@ -2130,16 +2182,34 @@
       <c r="Z31" s="3"/>
     </row>
     <row r="32">
-      <c r="A32" s="9"/>
-      <c r="B32" s="10"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
+      <c r="A32" s="9">
+        <v>27.0</v>
+      </c>
+      <c r="B32" s="10">
+        <v>45380.0</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>89</v>
+      </c>
       <c r="F32" s="3"/>
-      <c r="G32" s="9"/>
-      <c r="H32" s="9"/>
-      <c r="I32" s="3"/>
-      <c r="J32" s="3"/>
+      <c r="G32" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="H32" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="I32" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="J32" s="9" t="s">
+        <v>132</v>
+      </c>
       <c r="K32" s="3"/>
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
@@ -2158,16 +2228,36 @@
       <c r="Z32" s="3"/>
     </row>
     <row r="33">
-      <c r="A33" s="3"/>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
-      <c r="I33" s="3"/>
-      <c r="J33" s="3"/>
+      <c r="A33" s="9">
+        <v>28.0</v>
+      </c>
+      <c r="B33" s="12">
+        <v>45391.0</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="F33" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G33" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="H33" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="I33" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="J33" s="9" t="s">
+        <v>136</v>
+      </c>
       <c r="K33" s="3"/>
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
@@ -2186,16 +2276,36 @@
       <c r="Z33" s="3"/>
     </row>
     <row r="34">
-      <c r="A34" s="3"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="3"/>
-      <c r="H34" s="3"/>
-      <c r="I34" s="3"/>
-      <c r="J34" s="3"/>
+      <c r="A34" s="9">
+        <v>29.0</v>
+      </c>
+      <c r="B34" s="12">
+        <v>45391.0</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="F34" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G34" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="H34" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="I34" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="J34" s="9" t="s">
+        <v>140</v>
+      </c>
       <c r="K34" s="3"/>
       <c r="L34" s="3"/>
       <c r="M34" s="3"/>
@@ -2214,16 +2324,36 @@
       <c r="Z34" s="3"/>
     </row>
     <row r="35">
-      <c r="A35" s="3"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
-      <c r="H35" s="3"/>
-      <c r="I35" s="3"/>
-      <c r="J35" s="3"/>
+      <c r="A35" s="9">
+        <v>30.0</v>
+      </c>
+      <c r="B35" s="12">
+        <v>45391.0</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="F35" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G35" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="H35" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="I35" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="J35" s="9" t="s">
+        <v>144</v>
+      </c>
       <c r="K35" s="3"/>
       <c r="L35" s="3"/>
       <c r="M35" s="3"/>

</xml_diff>

<commit_message>
Revert "Merge origin/main into feature/levels"
This reverts commit 0c75ae794e348273deed1f30d11d89534575c8bc.
</commit_message>
<xml_diff>
--- a/doc/bug-report.xlsx
+++ b/doc/bug-report.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="129">
   <si>
     <t>P0 = crash bug, P1 = game stopping but not crash, P2 = not working as expected, P3 = annoying, P4 = nice to have, P5 = future release</t>
   </si>
@@ -401,62 +401,13 @@
   <si>
     <t>add "delete root" inside of the decision tree destructor, open game, close game, error</t>
   </si>
-  <si>
-    <t>mesh collider not working, box collidable is smaller than mesh, so it won't ever check against mesh</t>
-  </si>
-  <si>
-    <t>bullets passing through mesh should hit the player</t>
-  </si>
-  <si>
-    <t>bullets should damage player when passing through mesh collider</t>
-  </si>
-  <si>
-    <t>press g for debug, let enemy shoot you, dodge by going down while letting bullet grace top half of mesh -&gt; not hitting</t>
-  </si>
-  <si>
-    <t>Sometimes the fog of war does not reveal the entire room</t>
-  </si>
-  <si>
-    <t>Entering a room reveals the entire room</t>
-  </si>
-  <si>
-    <t>Occasionally a corner of the room will be hidden in a triangle shape of shadows. Entering the triangle reveals it as normal</t>
-  </si>
-  <si>
-    <t>Generate a room and corridor such that a door is facing vertically is directly next to a door facing horizontally into the other door. The corresponding room will have the fog bug.</t>
-  </si>
-  <si>
-    <t>Sometimes only three enemies will spawn inside a room causing the player to be stuck in that room as they cannot kill the fourth enemy.</t>
-  </si>
-  <si>
-    <t>All four enemies should be inside a room and interactable.</t>
-  </si>
-  <si>
-    <t>An enemy will be missing in a room in some generations.</t>
-  </si>
-  <si>
-    <t>Keep generating and entering rooms until only 3 enemies are accessable.</t>
-  </si>
-  <si>
-    <t>Game crashing when player's room index is -1 which means its in a corridor, so the array access is invalid</t>
-  </si>
-  <si>
-    <t>the game should not crash</t>
-  </si>
-  <si>
-    <t>game crashes</t>
-  </si>
-  <si>
-    <t>[not able to reproduce]</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
-    <numFmt numFmtId="165" formatCode="mm/dd/yyyy"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -513,7 +464,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -549,9 +500,6 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1716,7 +1664,7 @@
         <v>88</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>74</v>
+        <v>13</v>
       </c>
       <c r="E22" s="9" t="s">
         <v>89</v>
@@ -2182,34 +2130,16 @@
       <c r="Z31" s="3"/>
     </row>
     <row r="32">
-      <c r="A32" s="9">
-        <v>27.0</v>
-      </c>
-      <c r="B32" s="10">
-        <v>45380.0</v>
-      </c>
-      <c r="C32" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="E32" s="9" t="s">
-        <v>89</v>
-      </c>
+      <c r="A32" s="9"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
       <c r="F32" s="3"/>
-      <c r="G32" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="H32" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="I32" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="J32" s="9" t="s">
-        <v>132</v>
-      </c>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
       <c r="K32" s="3"/>
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
@@ -2228,36 +2158,16 @@
       <c r="Z32" s="3"/>
     </row>
     <row r="33">
-      <c r="A33" s="9">
-        <v>28.0</v>
-      </c>
-      <c r="B33" s="12">
-        <v>45391.0</v>
-      </c>
-      <c r="C33" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D33" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="E33" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="F33" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G33" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="H33" s="9" t="s">
-        <v>134</v>
-      </c>
-      <c r="I33" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="J33" s="9" t="s">
-        <v>136</v>
-      </c>
+      <c r="A33" s="3"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
       <c r="K33" s="3"/>
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
@@ -2276,36 +2186,16 @@
       <c r="Z33" s="3"/>
     </row>
     <row r="34">
-      <c r="A34" s="9">
-        <v>29.0</v>
-      </c>
-      <c r="B34" s="12">
-        <v>45391.0</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E34" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="F34" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G34" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="H34" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="I34" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="J34" s="9" t="s">
-        <v>140</v>
-      </c>
+      <c r="A34" s="3"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
       <c r="K34" s="3"/>
       <c r="L34" s="3"/>
       <c r="M34" s="3"/>
@@ -2324,36 +2214,16 @@
       <c r="Z34" s="3"/>
     </row>
     <row r="35">
-      <c r="A35" s="9">
-        <v>30.0</v>
-      </c>
-      <c r="B35" s="12">
-        <v>45391.0</v>
-      </c>
-      <c r="C35" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D35" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E35" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="F35" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G35" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="H35" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="I35" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="J35" s="9" t="s">
-        <v>144</v>
-      </c>
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
       <c r="K35" s="3"/>
       <c r="L35" s="3"/>
       <c r="M35" s="3"/>

</xml_diff>